<commit_message>
Tweeked a bunch of little features
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/outfits_sheet.xlsx
+++ b/assets/spreadsheets/outfits_sheet.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jayden\PycharmProjects\pythonProject1\assets\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAA07E5-8535-482F-B89A-5D1AA2AE4DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1F4448-30EC-4A58-826A-DEB3B8021AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-360" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="outfits_sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Maggie" sheetId="3" r:id="rId1"/>
     <sheet name="outfits_sheet (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -329,19 +329,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF3DA78-9348-467C-8CDD-C77F93FAE69C}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -400,21 +400,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>